<commit_message>
Add AutoCAD TakeOff Wizard and 3D viewer to project
Consolidates the AutoCAD LISP takeoff tool (T24_TakeOff.lsp, tz_to_excel.py)
and the 3D building viewer (viewer.html, viewer_server.py) into the main
T24 Streamline repo. Updates README with unified workflow documentation.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/T24 Input Template.xlsx
+++ b/T24 Input Template.xlsx
@@ -686,7 +686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,7 +784,6 @@
           <t>R-21 Wood Framed Wall</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -820,7 +819,6 @@
           <t>R-21 Wood Framed Wall</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -856,7 +854,6 @@
           <t>R-21 Wood Framed Wall</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -879,7 +876,11 @@
           <t>Interior Wall</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>West</t>
+        </is>
+      </c>
       <c r="F5" t="n">
         <v>220</v>
       </c>
@@ -915,7 +916,6 @@
           <t>Roof</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>651</v>
       </c>
@@ -924,7 +924,6 @@
           <t>R-38 Roof</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -947,7 +946,6 @@
           <t>Slab on Grade</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>651</v>
       </c>
@@ -956,10 +954,186 @@
           <t>Slab-on-Grade</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>W-102-N</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>W-102-S</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Z-102</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>South Wall</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Exterior Wall</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>South</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>240</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>R-21 Wood Framed Wall</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>W-102-W</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Z-102</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>West Wall</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Exterior Wall</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>West</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>240</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>R-21 Wood Framed Wall</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>W-102-DM</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Z-102</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Demising</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Interior Wall</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>East</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>240</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>R-0 Wall</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Z-101</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>W-102-RF</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Z-102</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Roof</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Roof</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>900</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>R-38 Roof</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>W-102-SL</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Z-102</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Slab</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Slab on Grade</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>900</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Slab-on-Grade</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
         <is>
           <t># Gross Area = total wall area INCLUDING windows/doors. Orientation required for exterior walls.</t>
         </is>
@@ -979,7 +1153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1155,10 +1329,78 @@
       <c r="F5" t="n">
         <v>0.5</v>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>O-102-N-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>O-102-S-1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>W-102-S</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>South Window</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>48</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>O-102-W-1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>W-102-W</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>West Window</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>24</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t># U-Factor and SHGC required for windows; leave blank for doors.</t>
         </is>

</xml_diff>